<commit_message>
Regenerated SML IG outputs following improvements to patient profiles
Added a number of invariants to 3 patient profiles and some narrative updates.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medication-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/medication-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$75</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="367">
   <si>
     <t>Path</t>
   </si>
@@ -583,22 +583,29 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t>Medication.code.coding.extension.valueCoding</t>
+    <t>Medication.code.coding.extension.value[x]</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Extension.value[x]</t>
   </si>
   <si>
     <t>valueCoding</t>
   </si>
   <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
-  </si>
-  <si>
     <t>http://hl7.org.au/fhir/ValueSet/medication-type</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
   </si>
   <si>
     <t>Medication.code.coding.system</t>
@@ -941,9 +948,6 @@
     <t>RXC-2-Component Code  if medication: RXO-1-Requested Give Code / RXE-2-Give Code / RXD-2-Dispense/Give Code / RXG-4-Give Code / RXA-5-Administered Code</t>
   </si>
   <si>
-    <t>Medication.ingredient.itemCodeableConcept</t>
-  </si>
-  <si>
     <t>itemCodeableConcept</t>
   </si>
   <si>
@@ -953,13 +957,13 @@
     <t>Coding for a substance or medicinal product  that is an ingredient of the medication.</t>
   </si>
   <si>
-    <t>Medication.ingredient.itemCodeableConcept.id</t>
-  </si>
-  <si>
-    <t>Medication.ingredient.itemCodeableConcept.extension</t>
-  </si>
-  <si>
-    <t>Medication.ingredient.itemCodeableConcept.coding</t>
+    <t>Medication.ingredient.item[x].id</t>
+  </si>
+  <si>
+    <t>Medication.ingredient.item[x].extension</t>
+  </si>
+  <si>
+    <t>Medication.ingredient.item[x].coding</t>
   </si>
   <si>
     <t>amtMP</t>
@@ -971,7 +975,7 @@
     <t>http://hl7.org.au/fhir/ValueSet/amt-mp-codes</t>
   </si>
   <si>
-    <t>Medication.ingredient.itemCodeableConcept.text</t>
+    <t>Medication.ingredient.item[x].text</t>
   </si>
   <si>
     <t>Medication.ingredient.isActive</t>
@@ -1312,7 +1316,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM74"/>
+  <dimension ref="A1:AM75"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1321,7 +1325,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.6953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.48828125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="20.9296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -4139,15 +4143,13 @@
       <c r="A26" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="B26" t="s" s="2">
-        <v>178</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>50</v>
@@ -4165,10 +4167,10 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>180</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4195,28 +4197,26 @@
         <v>40</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="Y26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA26" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AB26" s="2"/>
+      <c r="AC26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD26" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="Z26" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA26" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB26" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC26" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD26" t="s" s="2">
-        <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
         <v>182</v>
@@ -4248,15 +4248,17 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>50</v>
@@ -4268,23 +4270,19 @@
         <v>40</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>63</v>
+        <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>187</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>40</v>
       </c>
@@ -4308,13 +4306,13 @@
         <v>40</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4332,7 +4330,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4350,18 +4348,18 @@
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>189</v>
+        <v>93</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4384,18 +4382,20 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="N28" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="N28" t="s" s="2">
+        <v>189</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>40</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4461,18 +4461,18 @@
         <v>40</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4495,18 +4495,18 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" t="s" s="2">
-        <v>201</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>40</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4572,18 +4572,18 @@
         <v>40</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4606,17 +4606,17 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>40</v>
@@ -4665,7 +4665,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4683,18 +4683,18 @@
         <v>40</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4717,19 +4717,17 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>216</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" t="s" s="2">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>40</v>
@@ -4778,7 +4776,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -4796,22 +4794,20 @@
         <v>40</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="B32" t="s" s="2">
-        <v>221</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
         <v>40</v>
       </c>
@@ -4832,19 +4828,19 @@
         <v>51</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>142</v>
+        <v>215</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>144</v>
+        <v>217</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>145</v>
+        <v>218</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>40</v>
@@ -4869,11 +4865,13 @@
         <v>40</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X32" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y32" t="s" s="2">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>40</v>
@@ -4891,13 +4889,13 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>40</v>
@@ -4909,20 +4907,22 @@
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>150</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="B33" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>223</v>
+      </c>
       <c r="C33" t="s" s="2">
         <v>40</v>
       </c>
@@ -4943,19 +4943,19 @@
         <v>51</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>226</v>
+        <v>144</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>40</v>
@@ -4980,13 +4980,11 @@
         <v>40</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>40</v>
+        <v>225</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>40</v>
@@ -5004,13 +5002,13 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>229</v>
+        <v>148</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>40</v>
@@ -5022,18 +5020,18 @@
         <v>40</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>230</v>
+        <v>149</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>231</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5056,18 +5054,20 @@
         <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N34" s="2"/>
+        <v>229</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>40</v>
       </c>
@@ -5091,13 +5091,13 @@
         <v>40</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -5115,36 +5115,36 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK34" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="AF34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>238</v>
-      </c>
       <c r="AL34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>40</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5167,15 +5167,17 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>213</v>
+        <v>69</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="M35" s="2"/>
+        <v>236</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>237</v>
+      </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>40</v>
@@ -5200,13 +5202,13 @@
         <v>40</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>40</v>
+        <v>239</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>40</v>
@@ -5224,7 +5226,7 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5239,13 +5241,13 @@
         <v>40</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>40</v>
@@ -5253,7 +5255,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5276,13 +5278,13 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5333,25 +5335,25 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="AF36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="AK36" t="s" s="2">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>128</v>
@@ -5360,9 +5362,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5376,7 +5378,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>40</v>
@@ -5385,13 +5387,13 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5442,7 +5444,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5457,21 +5459,21 @@
         <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>253</v>
+        <v>128</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>254</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5491,20 +5493,18 @@
         <v>40</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>118</v>
+        <v>251</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>258</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5529,13 +5529,13 @@
         <v>40</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>260</v>
+        <v>40</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>40</v>
@@ -5553,36 +5553,36 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AF38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="AM38" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5596,7 +5596,7 @@
         <v>50</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>40</v>
@@ -5605,15 +5605,17 @@
         <v>40</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>259</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5638,13 +5640,13 @@
         <v>40</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>40</v>
@@ -5662,7 +5664,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5677,32 +5679,32 @@
         <v>40</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>40</v>
+        <v>263</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>40</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>40</v>
@@ -5714,17 +5716,15 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5761,25 +5761,25 @@
         <v>40</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="AC40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD40" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>40</v>
@@ -5802,18 +5802,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>40</v>
@@ -5822,23 +5822,21 @@
         <v>40</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5874,9 +5872,11 @@
         <v>40</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="AB41" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>139</v>
+      </c>
       <c r="AC41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>99</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5902,22 +5902,20 @@
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="B42" t="s" s="2">
         <v>268</v>
       </c>
+      <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>40</v>
       </c>
@@ -5941,7 +5939,7 @@
         <v>142</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>269</v>
+        <v>143</v>
       </c>
       <c r="L42" t="s" s="2">
         <v>144</v>
@@ -5975,26 +5973,26 @@
         <v>40</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X42" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y42" t="s" s="2">
-        <v>270</v>
+        <v>40</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AA42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="AB42" s="2"/>
       <c r="AC42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD42" t="s" s="2">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="AE42" t="s" s="2">
         <v>148</v>
@@ -6026,9 +6024,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="B43" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>270</v>
+      </c>
       <c r="C43" t="s" s="2">
         <v>40</v>
       </c>
@@ -6049,19 +6049,19 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>273</v>
+        <v>144</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
@@ -6086,13 +6086,11 @@
         <v>40</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X43" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X43" s="2"/>
       <c r="Y43" t="s" s="2">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>40</v>
@@ -6110,13 +6108,13 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>229</v>
+        <v>148</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
@@ -6128,18 +6126,18 @@
         <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>230</v>
+        <v>149</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>231</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6150,30 +6148,32 @@
         <v>41</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I44" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I44" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J44" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="K44" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>277</v>
-      </c>
       <c r="M44" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="N44" s="2"/>
+        <v>229</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>40</v>
       </c>
@@ -6221,36 +6221,36 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>279</v>
+        <v>40</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>280</v>
+        <v>232</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>40</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="45" hidden="true">
+    <row r="45">
       <c r="A45" t="s" s="2">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6261,10 +6261,10 @@
         <v>41</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>40</v>
@@ -6273,15 +6273,17 @@
         <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>132</v>
+        <v>278</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M45" s="2"/>
+        <v>279</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6330,25 +6332,25 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>134</v>
+        <v>276</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>135</v>
+        <v>282</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>40</v>
@@ -6359,18 +6361,18 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>40</v>
@@ -6382,17 +6384,15 @@
         <v>40</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>40</v>
@@ -6441,13 +6441,13 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>40</v>
@@ -6470,11 +6470,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>284</v>
+        <v>112</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6487,19 +6487,19 @@
         <v>40</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J47" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>285</v>
+        <v>138</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>115</v>
@@ -6552,7 +6552,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>286</v>
+        <v>140</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6570,7 +6570,7 @@
         <v>40</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>40</v>
@@ -6579,40 +6579,42 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H48" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H48" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="I48" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>288</v>
+        <v>95</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>289</v>
+        <v>113</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="M48" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>40</v>
@@ -6661,13 +6663,13 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>40</v>
@@ -6676,25 +6678,23 @@
         <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>291</v>
+        <v>93</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>292</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>294</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>40</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>50</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>40</v>
@@ -6715,13 +6715,13 @@
         <v>40</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>118</v>
+        <v>290</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6760,19 +6760,17 @@
         <v>40</v>
       </c>
       <c r="AA49" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="AB49" s="2"/>
       <c r="AC49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD49" t="s" s="2">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>50</v>
@@ -6790,26 +6788,28 @@
         <v>126</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="B50" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>295</v>
+      </c>
       <c r="C50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>50</v>
@@ -6824,13 +6824,13 @@
         <v>40</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>132</v>
+        <v>296</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>133</v>
+        <v>297</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6881,10 +6881,10 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>134</v>
+        <v>289</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>50</v>
@@ -6896,16 +6896,16 @@
         <v>40</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>135</v>
+        <v>293</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>40</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -6914,14 +6914,14 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>40</v>
@@ -6933,17 +6933,15 @@
         <v>40</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>40</v>
@@ -6980,25 +6978,25 @@
         <v>40</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>40</v>
@@ -7025,7 +7023,7 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7041,23 +7039,21 @@
         <v>40</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>40</v>
       </c>
@@ -7093,9 +7089,11 @@
         <v>40</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="AB52" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>139</v>
+      </c>
       <c r="AC52" t="s" s="2">
         <v>40</v>
       </c>
@@ -7103,7 +7101,7 @@
         <v>99</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7121,22 +7119,20 @@
         <v>40</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="B53" t="s" s="2">
         <v>300</v>
       </c>
+      <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
         <v>40</v>
       </c>
@@ -7145,7 +7141,7 @@
         <v>41</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>40</v>
@@ -7160,7 +7156,7 @@
         <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>301</v>
+        <v>143</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>144</v>
@@ -7194,26 +7190,26 @@
         <v>40</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X53" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y53" t="s" s="2">
-        <v>302</v>
+        <v>40</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="AB53" s="2"/>
       <c r="AC53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD53" t="s" s="2">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="AE53" t="s" s="2">
         <v>148</v>
@@ -7245,9 +7241,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="B54" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="C54" t="s" s="2">
         <v>40</v>
       </c>
@@ -7268,19 +7266,19 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>273</v>
+        <v>144</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
@@ -7305,13 +7303,11 @@
         <v>40</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X54" s="2"/>
       <c r="Y54" t="s" s="2">
-        <v>40</v>
+        <v>303</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>40</v>
@@ -7329,13 +7325,13 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>229</v>
+        <v>148</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>40</v>
@@ -7347,16 +7343,16 @@
         <v>40</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>230</v>
+        <v>149</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>231</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
         <v>304</v>
       </c>
@@ -7372,26 +7368,28 @@
         <v>50</v>
       </c>
       <c r="G55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I55" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="J55" t="s" s="2">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="M55" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>229</v>
+      </c>
       <c r="N55" t="s" s="2">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
@@ -7440,7 +7438,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>304</v>
+        <v>231</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7458,18 +7456,18 @@
         <v>40</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>40</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7492,16 +7490,18 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+      <c r="N56" t="s" s="2">
+        <v>308</v>
+      </c>
       <c r="O56" t="s" s="2">
         <v>40</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7564,21 +7564,21 @@
         <v>40</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>312</v>
+        <v>40</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>313</v>
+        <v>249</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>314</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7601,13 +7601,13 @@
         <v>40</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7658,36 +7658,36 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="AF57" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG57" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH57" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI57" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AJ57" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>40</v>
-      </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7701,7 +7701,7 @@
         <v>50</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>40</v>
@@ -7710,13 +7710,13 @@
         <v>40</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>132</v>
+        <v>317</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>133</v>
+        <v>318</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7767,7 +7767,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>134</v>
+        <v>316</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7779,13 +7779,13 @@
         <v>40</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>40</v>
+        <v>244</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>135</v>
+        <v>319</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
@@ -7800,14 +7800,14 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>40</v>
@@ -7819,17 +7819,15 @@
         <v>40</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -7878,13 +7876,13 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>40</v>
@@ -7911,7 +7909,7 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>284</v>
+        <v>112</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -7924,19 +7922,19 @@
         <v>40</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J60" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>285</v>
+        <v>138</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>115</v>
@@ -7989,7 +7987,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>286</v>
+        <v>140</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8007,7 +8005,7 @@
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
@@ -8022,34 +8020,36 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>323</v>
+        <v>113</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="M61" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>40</v>
@@ -8074,13 +8074,13 @@
         <v>40</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>326</v>
+        <v>40</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>40</v>
@@ -8098,13 +8098,13 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>40</v>
@@ -8113,10 +8113,10 @@
         <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>40</v>
@@ -8127,7 +8127,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8138,7 +8138,7 @@
         <v>41</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>40</v>
@@ -8150,13 +8150,13 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>275</v>
+        <v>118</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8183,13 +8183,13 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>40</v>
+        <v>326</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>40</v>
+        <v>327</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>40</v>
@@ -8207,25 +8207,25 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>279</v>
+        <v>40</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>330</v>
+        <v>127</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
@@ -8236,7 +8236,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8247,7 +8247,7 @@
         <v>41</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>40</v>
@@ -8259,13 +8259,13 @@
         <v>40</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>132</v>
+        <v>329</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>133</v>
+        <v>330</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8316,25 +8316,25 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>134</v>
+        <v>328</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>40</v>
+        <v>244</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>135</v>
+        <v>331</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
@@ -8349,14 +8349,14 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>40</v>
@@ -8368,17 +8368,15 @@
         <v>40</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>40</v>
@@ -8427,13 +8425,13 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>40</v>
@@ -8460,7 +8458,7 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>284</v>
+        <v>112</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
@@ -8473,19 +8471,19 @@
         <v>40</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J65" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>285</v>
+        <v>138</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>115</v>
@@ -8538,7 +8536,7 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>286</v>
+        <v>140</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8556,7 +8554,7 @@
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -8571,34 +8569,36 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>335</v>
+        <v>95</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>336</v>
+        <v>113</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="M66" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
@@ -8647,13 +8647,13 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>334</v>
+        <v>288</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
@@ -8662,10 +8662,10 @@
         <v>40</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>291</v>
+        <v>93</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
@@ -8676,7 +8676,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8684,7 +8684,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F67" t="s" s="2">
         <v>50</v>
@@ -8699,13 +8699,13 @@
         <v>40</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8756,10 +8756,10 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>50</v>
@@ -8771,10 +8771,10 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>40</v>
@@ -8783,9 +8783,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8799,7 +8799,7 @@
         <v>50</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>40</v>
@@ -8808,13 +8808,13 @@
         <v>40</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>275</v>
+        <v>340</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8865,25 +8865,25 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>279</v>
+        <v>40</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>345</v>
+        <v>314</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>40</v>
@@ -8892,9 +8892,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" hidden="true">
+    <row r="69">
       <c r="A69" t="s" s="2">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8908,7 +8908,7 @@
         <v>50</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H69" t="s" s="2">
         <v>40</v>
@@ -8917,13 +8917,13 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>132</v>
+        <v>344</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>133</v>
+        <v>345</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -8974,25 +8974,25 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>134</v>
+        <v>343</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>40</v>
+        <v>244</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>135</v>
+        <v>346</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9007,14 +9007,14 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>40</v>
@@ -9026,17 +9026,15 @@
         <v>40</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>40</v>
@@ -9085,13 +9083,13 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
@@ -9118,7 +9116,7 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>284</v>
+        <v>112</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9131,19 +9129,19 @@
         <v>40</v>
       </c>
       <c r="H71" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I71" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J71" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>285</v>
+        <v>138</v>
       </c>
       <c r="M71" t="s" s="2">
         <v>115</v>
@@ -9196,7 +9194,7 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>286</v>
+        <v>140</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9214,7 +9212,7 @@
         <v>40</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
@@ -9223,40 +9221,42 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
         <v>349</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G72" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H72" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H72" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="I72" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>350</v>
+        <v>113</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M72" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>40</v>
@@ -9305,13 +9305,13 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>349</v>
+        <v>288</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>40</v>
@@ -9320,21 +9320,21 @@
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>242</v>
+        <v>40</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>352</v>
+        <v>93</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>353</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9357,13 +9357,13 @@
         <v>40</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>355</v>
+        <v>131</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9414,36 +9414,36 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AF73" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG73" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM73" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="AF73" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>359</v>
-      </c>
     </row>
-    <row r="74" hidden="true">
+    <row r="74">
       <c r="A74" t="s" s="2">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9454,10 +9454,10 @@
         <v>41</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>40</v>
@@ -9466,18 +9466,16 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="M74" s="2"/>
-      <c r="N74" t="s" s="2">
-        <v>364</v>
-      </c>
+      <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
         <v>40</v>
       </c>
@@ -9525,35 +9523,146 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AK74" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="AL74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM74" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="AF74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG74" t="s" s="2">
+    </row>
+    <row r="75" hidden="true">
+      <c r="A75" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F75" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AH74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK74" t="s" s="2">
+      <c r="G75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J75" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="K75" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L75" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="M75" s="2"/>
+      <c r="N75" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="AL74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM74" t="s" s="2">
+      <c r="O75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P75" s="2"/>
+      <c r="Q75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE75" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AF75" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG75" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK75" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="AL75" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM74">
+  <autoFilter ref="A1:AM75">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9563,7 +9672,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI73">
+  <conditionalFormatting sqref="A2:AI74">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated outputs for SML with regards to a change in inv.dh-relper.01 to "At least one related person identifier shall at least have a system and a value"
CIFMM-2735
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medication-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/medication-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$74</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="366">
   <si>
     <t>Path</t>
   </si>
@@ -583,7 +583,10 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t>Medication.code.coding.extension.value[x]</t>
+    <t>Medication.code.coding.extension.valueCoding</t>
+  </si>
+  <si>
+    <t>valueCoding</t>
   </si>
   <si>
     <t>Value of extension</t>
@@ -592,20 +595,10 @@
     <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
   </si>
   <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
+    <t>http://hl7.org.au/fhir/ValueSet/medication-type</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>valueCoding</t>
-  </si>
-  <si>
-    <t>http://hl7.org.au/fhir/ValueSet/medication-type</t>
   </si>
   <si>
     <t>Medication.code.coding.system</t>
@@ -948,6 +941,9 @@
     <t>RXC-2-Component Code  if medication: RXO-1-Requested Give Code / RXE-2-Give Code / RXD-2-Dispense/Give Code / RXG-4-Give Code / RXA-5-Administered Code</t>
   </si>
   <si>
+    <t>Medication.ingredient.itemCodeableConcept</t>
+  </si>
+  <si>
     <t>itemCodeableConcept</t>
   </si>
   <si>
@@ -957,13 +953,13 @@
     <t>Coding for a substance or medicinal product  that is an ingredient of the medication.</t>
   </si>
   <si>
-    <t>Medication.ingredient.item[x].id</t>
-  </si>
-  <si>
-    <t>Medication.ingredient.item[x].extension</t>
-  </si>
-  <si>
-    <t>Medication.ingredient.item[x].coding</t>
+    <t>Medication.ingredient.itemCodeableConcept.id</t>
+  </si>
+  <si>
+    <t>Medication.ingredient.itemCodeableConcept.extension</t>
+  </si>
+  <si>
+    <t>Medication.ingredient.itemCodeableConcept.coding</t>
   </si>
   <si>
     <t>amtMP</t>
@@ -975,7 +971,7 @@
     <t>http://hl7.org.au/fhir/ValueSet/amt-mp-codes</t>
   </si>
   <si>
-    <t>Medication.ingredient.item[x].text</t>
+    <t>Medication.ingredient.itemCodeableConcept.text</t>
   </si>
   <si>
     <t>Medication.ingredient.isActive</t>
@@ -1316,7 +1312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM75"/>
+  <dimension ref="A1:AM74"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1325,7 +1321,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.48828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.6953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="20.9296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -4143,13 +4139,15 @@
       <c r="A26" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" t="s" s="2">
+        <v>178</v>
+      </c>
       <c r="C26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>50</v>
@@ -4167,10 +4165,10 @@
         <v>142</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4197,26 +4195,28 @@
         <v>40</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AA26" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="AB26" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB26" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD26" t="s" s="2">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
         <v>182</v>
@@ -4248,17 +4248,15 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="B27" t="s" s="2">
         <v>183</v>
       </c>
+      <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>50</v>
@@ -4270,19 +4268,23 @@
         <v>40</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>142</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+        <v>185</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>187</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>40</v>
       </c>
@@ -4306,13 +4308,13 @@
         <v>40</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4330,7 +4332,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4348,18 +4350,18 @@
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>40</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4382,20 +4384,18 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>189</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>40</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4461,18 +4461,18 @@
         <v>40</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4495,18 +4495,18 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" t="s" s="2">
+        <v>201</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>40</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4572,18 +4572,18 @@
         <v>40</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4606,17 +4606,17 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>40</v>
@@ -4665,7 +4665,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4683,18 +4683,18 @@
         <v>40</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4717,17 +4717,19 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>131</v>
+        <v>213</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>215</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>216</v>
+      </c>
       <c r="N31" t="s" s="2">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>40</v>
@@ -4776,7 +4778,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -4794,20 +4796,22 @@
         <v>40</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>221</v>
+      </c>
       <c r="C32" t="s" s="2">
         <v>40</v>
       </c>
@@ -4828,19 +4832,19 @@
         <v>51</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>215</v>
+        <v>142</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>219</v>
+        <v>146</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>40</v>
@@ -4865,13 +4869,11 @@
         <v>40</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X32" s="2"/>
       <c r="Y32" t="s" s="2">
-        <v>40</v>
+        <v>223</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>40</v>
@@ -4889,13 +4891,13 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>40</v>
@@ -4907,22 +4909,20 @@
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>222</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="B33" t="s" s="2">
-        <v>223</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
         <v>40</v>
       </c>
@@ -4943,19 +4943,19 @@
         <v>51</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>40</v>
@@ -4980,11 +4980,13 @@
         <v>40</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X33" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y33" t="s" s="2">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>40</v>
@@ -5002,13 +5004,13 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>40</v>
@@ -5020,18 +5022,18 @@
         <v>40</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>150</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5054,20 +5056,18 @@
         <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>40</v>
       </c>
@@ -5091,13 +5091,13 @@
         <v>40</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>40</v>
+        <v>236</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -5115,7 +5115,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5133,18 +5133,18 @@
         <v>40</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>233</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5167,17 +5167,15 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>69</v>
+        <v>213</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>237</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>40</v>
@@ -5202,32 +5200,32 @@
         <v>40</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>238</v>
+        <v>40</v>
       </c>
       <c r="Y35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE35" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="Z35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>234</v>
-      </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
       </c>
@@ -5241,13 +5239,13 @@
         <v>40</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>40</v>
@@ -5255,7 +5253,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5278,13 +5276,13 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5335,7 +5333,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5350,10 +5348,10 @@
         <v>40</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>128</v>
@@ -5362,9 +5360,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5378,7 +5376,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>40</v>
@@ -5387,13 +5385,13 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5444,7 +5442,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5459,21 +5457,21 @@
         <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>128</v>
+        <v>253</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5493,18 +5491,20 @@
         <v>40</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>251</v>
+        <v>118</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M38" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>258</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5529,13 +5529,13 @@
         <v>40</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>40</v>
+        <v>260</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>40</v>
@@ -5553,7 +5553,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5568,21 +5568,21 @@
         <v>40</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>255</v>
+        <v>40</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5596,7 +5596,7 @@
         <v>50</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>40</v>
@@ -5605,17 +5605,15 @@
         <v>40</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>258</v>
+        <v>132</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>260</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5640,13 +5638,13 @@
         <v>40</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>261</v>
+        <v>40</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>262</v>
+        <v>40</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>40</v>
@@ -5664,7 +5662,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>257</v>
+        <v>134</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5679,32 +5677,32 @@
         <v>40</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>263</v>
+        <v>40</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>264</v>
+        <v>135</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>265</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>40</v>
@@ -5716,15 +5714,17 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M40" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5761,25 +5761,25 @@
         <v>40</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="AC40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD40" t="s" s="2">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>40</v>
@@ -5802,18 +5802,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>40</v>
@@ -5822,21 +5822,23 @@
         <v>40</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="N41" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>146</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5872,11 +5874,9 @@
         <v>40</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>139</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="AB41" s="2"/>
       <c r="AC41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>99</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5902,20 +5902,22 @@
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>40</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="B42" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>40</v>
       </c>
@@ -5939,7 +5941,7 @@
         <v>142</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>143</v>
+        <v>269</v>
       </c>
       <c r="L42" t="s" s="2">
         <v>144</v>
@@ -5973,26 +5975,26 @@
         <v>40</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X42" s="2"/>
       <c r="Y42" t="s" s="2">
-        <v>40</v>
+        <v>270</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AA42" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AB42" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD42" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
         <v>148</v>
@@ -6024,11 +6026,9 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="B43" t="s" s="2">
-        <v>270</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
         <v>40</v>
       </c>
@@ -6049,19 +6049,19 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>144</v>
+        <v>273</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
@@ -6086,11 +6086,13 @@
         <v>40</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X43" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y43" t="s" s="2">
-        <v>272</v>
+        <v>40</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>40</v>
@@ -6108,13 +6110,13 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
@@ -6126,18 +6128,18 @@
         <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>150</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="44" hidden="true">
+    <row r="44">
       <c r="A44" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6148,32 +6150,30 @@
         <v>41</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>131</v>
+        <v>275</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>40</v>
       </c>
@@ -6221,36 +6221,36 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>233</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6261,10 +6261,10 @@
         <v>41</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>40</v>
@@ -6273,17 +6273,15 @@
         <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>277</v>
+        <v>131</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>278</v>
+        <v>132</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6332,25 +6330,25 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>276</v>
+        <v>134</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>282</v>
+        <v>135</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>40</v>
@@ -6361,18 +6359,18 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>40</v>
@@ -6384,15 +6382,17 @@
         <v>40</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M46" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>40</v>
@@ -6441,13 +6441,13 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>40</v>
@@ -6470,11 +6470,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>112</v>
+        <v>284</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6487,19 +6487,19 @@
         <v>40</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>115</v>
@@ -6552,7 +6552,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>140</v>
+        <v>286</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6570,7 +6570,7 @@
         <v>40</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>40</v>
@@ -6579,42 +6579,40 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>95</v>
+        <v>288</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>113</v>
+        <v>289</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>40</v>
@@ -6663,13 +6661,13 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>40</v>
@@ -6678,23 +6676,25 @@
         <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>40</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B49" s="2"/>
+        <v>293</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>294</v>
+      </c>
       <c r="C49" t="s" s="2">
         <v>40</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>50</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>40</v>
@@ -6715,13 +6715,13 @@
         <v>40</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>290</v>
+        <v>118</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6760,17 +6760,19 @@
         <v>40</v>
       </c>
       <c r="AA49" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="AB49" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD49" t="s" s="2">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>50</v>
@@ -6788,28 +6790,26 @@
         <v>126</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>295</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>50</v>
@@ -6824,13 +6824,13 @@
         <v>40</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>296</v>
+        <v>132</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>297</v>
+        <v>133</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6881,10 +6881,10 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>289</v>
+        <v>134</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>50</v>
@@ -6896,16 +6896,16 @@
         <v>40</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>293</v>
+        <v>135</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>294</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -6914,14 +6914,14 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>40</v>
@@ -6933,15 +6933,17 @@
         <v>40</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M51" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>40</v>
@@ -6978,25 +6980,25 @@
         <v>40</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>40</v>
@@ -7023,7 +7025,7 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7039,21 +7041,23 @@
         <v>40</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="N52" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>146</v>
+      </c>
       <c r="O52" t="s" s="2">
         <v>40</v>
       </c>
@@ -7089,11 +7093,9 @@
         <v>40</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>139</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="AB52" s="2"/>
       <c r="AC52" t="s" s="2">
         <v>40</v>
       </c>
@@ -7101,7 +7103,7 @@
         <v>99</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7119,20 +7121,22 @@
         <v>40</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>40</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="B53" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
         <v>40</v>
       </c>
@@ -7141,7 +7145,7 @@
         <v>41</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>40</v>
@@ -7156,7 +7160,7 @@
         <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>143</v>
+        <v>301</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>144</v>
@@ -7190,26 +7194,26 @@
         <v>40</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>40</v>
+        <v>302</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AB53" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD53" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
         <v>148</v>
@@ -7241,11 +7245,9 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
         <v>40</v>
       </c>
@@ -7266,19 +7268,19 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>144</v>
+        <v>273</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
@@ -7303,11 +7305,13 @@
         <v>40</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="X54" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y54" t="s" s="2">
-        <v>303</v>
+        <v>40</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>40</v>
@@ -7325,13 +7329,13 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>40</v>
@@ -7343,16 +7347,16 @@
         <v>40</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>150</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
         <v>304</v>
       </c>
@@ -7368,28 +7372,26 @@
         <v>50</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>131</v>
+        <v>213</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>229</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>230</v>
+        <v>307</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
@@ -7438,7 +7440,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>231</v>
+        <v>304</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7456,18 +7458,18 @@
         <v>40</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>233</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7490,18 +7492,16 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>215</v>
+        <v>309</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="M56" s="2"/>
-      <c r="N56" t="s" s="2">
-        <v>308</v>
-      </c>
+      <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>40</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7564,21 +7564,21 @@
         <v>40</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>40</v>
+        <v>312</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>249</v>
+        <v>313</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>40</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7601,13 +7601,13 @@
         <v>40</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7658,7 +7658,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7670,24 +7670,24 @@
         <v>40</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>313</v>
+        <v>242</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>315</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7701,7 +7701,7 @@
         <v>50</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>40</v>
@@ -7710,13 +7710,13 @@
         <v>40</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>277</v>
+        <v>131</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>317</v>
+        <v>132</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>318</v>
+        <v>133</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7767,7 +7767,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>316</v>
+        <v>134</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7779,13 +7779,13 @@
         <v>40</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>319</v>
+        <v>135</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
@@ -7800,14 +7800,14 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>40</v>
@@ -7819,15 +7819,17 @@
         <v>40</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M59" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -7876,13 +7878,13 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>40</v>
@@ -7909,7 +7911,7 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>112</v>
+        <v>284</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -7922,19 +7924,19 @@
         <v>40</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J60" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>115</v>
@@ -7987,7 +7989,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>140</v>
+        <v>286</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8005,7 +8007,7 @@
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
@@ -8020,36 +8022,34 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>113</v>
+        <v>323</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>40</v>
@@ -8074,13 +8074,13 @@
         <v>40</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>40</v>
+        <v>326</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>40</v>
@@ -8098,13 +8098,13 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>40</v>
@@ -8113,10 +8113,10 @@
         <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>40</v>
@@ -8127,7 +8127,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8138,7 +8138,7 @@
         <v>41</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>40</v>
@@ -8150,13 +8150,13 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>118</v>
+        <v>275</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8183,49 +8183,49 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>326</v>
+        <v>40</v>
       </c>
       <c r="Y62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE62" t="s" s="2">
         <v>327</v>
       </c>
-      <c r="Z62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>323</v>
-      </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>127</v>
+        <v>330</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
@@ -8236,7 +8236,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8247,7 +8247,7 @@
         <v>41</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>40</v>
@@ -8259,13 +8259,13 @@
         <v>40</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>277</v>
+        <v>131</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>329</v>
+        <v>132</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>330</v>
+        <v>133</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8316,25 +8316,25 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>328</v>
+        <v>134</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>331</v>
+        <v>135</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
@@ -8349,14 +8349,14 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>40</v>
@@ -8368,15 +8368,17 @@
         <v>40</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M64" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>40</v>
@@ -8425,13 +8427,13 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>40</v>
@@ -8458,7 +8460,7 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>112</v>
+        <v>284</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
@@ -8471,19 +8473,19 @@
         <v>40</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J65" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>115</v>
@@ -8536,7 +8538,7 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>140</v>
+        <v>286</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8554,7 +8556,7 @@
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -8569,36 +8571,34 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>95</v>
+        <v>335</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>113</v>
+        <v>336</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
@@ -8647,13 +8647,13 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>288</v>
+        <v>334</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
@@ -8662,10 +8662,10 @@
         <v>40</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
@@ -8676,7 +8676,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8684,7 +8684,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F67" t="s" s="2">
         <v>50</v>
@@ -8699,13 +8699,13 @@
         <v>40</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8756,10 +8756,10 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>50</v>
@@ -8771,10 +8771,10 @@
         <v>40</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>40</v>
@@ -8783,9 +8783,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" hidden="true">
+    <row r="68">
       <c r="A68" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8799,7 +8799,7 @@
         <v>50</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>40</v>
@@ -8808,13 +8808,13 @@
         <v>40</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>340</v>
+        <v>275</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8865,25 +8865,25 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>314</v>
+        <v>345</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>40</v>
@@ -8892,9 +8892,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8908,7 +8908,7 @@
         <v>50</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H69" t="s" s="2">
         <v>40</v>
@@ -8917,13 +8917,13 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>277</v>
+        <v>131</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>344</v>
+        <v>132</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>345</v>
+        <v>133</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -8974,25 +8974,25 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>343</v>
+        <v>134</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>346</v>
+        <v>135</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9007,14 +9007,14 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>40</v>
@@ -9026,15 +9026,17 @@
         <v>40</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M70" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>40</v>
@@ -9083,13 +9085,13 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
@@ -9116,7 +9118,7 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>112</v>
+        <v>284</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -9129,19 +9131,19 @@
         <v>40</v>
       </c>
       <c r="H71" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I71" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J71" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="M71" t="s" s="2">
         <v>115</v>
@@ -9194,7 +9196,7 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>140</v>
+        <v>286</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9212,7 +9214,7 @@
         <v>40</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
@@ -9221,42 +9223,40 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" hidden="true">
+    <row r="72">
       <c r="A72" t="s" s="2">
         <v>349</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>286</v>
+        <v>40</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H72" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I72" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>113</v>
+        <v>350</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>40</v>
@@ -9305,13 +9305,13 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>288</v>
+        <v>349</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>40</v>
@@ -9320,21 +9320,21 @@
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>93</v>
+        <v>352</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>40</v>
+        <v>353</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9357,13 +9357,13 @@
         <v>40</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>131</v>
+        <v>355</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9414,7 +9414,7 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9429,21 +9429,21 @@
         <v>40</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9454,10 +9454,10 @@
         <v>41</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>40</v>
@@ -9466,16 +9466,18 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
+      <c r="N74" t="s" s="2">
+        <v>364</v>
+      </c>
       <c r="O74" t="s" s="2">
         <v>40</v>
       </c>
@@ -9523,13 +9525,13 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH74" t="s" s="2">
         <v>40</v>
@@ -9538,131 +9540,20 @@
         <v>40</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="75" hidden="true">
-      <c r="A75" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F75" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M75" s="2"/>
-      <c r="N75" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P75" s="2"/>
-      <c r="Q75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM75" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM75">
+  <autoFilter ref="A1:AM74">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9672,7 +9563,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI74">
+  <conditionalFormatting sqref="A2:AI73">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerated SML FHIR IG outputs - for FHIRPath bugfix in SML List profile
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medication-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/medication-dh-base-1.xlsx
@@ -883,18 +883,6 @@
     <t>RXC-2-Component Code  if medication: RXO-1-Requested Give Code / RXE-2-Give Code / RXD-2-Dispense/Give Code / RXG-4-Give Code / RXA-5-Administered Code</t>
   </si>
   <si>
-    <t>itemCodeableConcept</t>
-  </si>
-  <si>
-    <t>Coded Ingredient Product</t>
-  </si>
-  <si>
-    <t>Coding for a substance or medicinal product  that is an ingredient of the medication.</t>
-  </si>
-  <si>
-    <t>http://hl7.org.au/fhir/ValueSet/amt-mp-codes</t>
-  </si>
-  <si>
     <t>itemReference</t>
   </si>
   <si>
@@ -903,6 +891,18 @@
   </si>
   <si>
     <t>Item Reference</t>
+  </si>
+  <si>
+    <t>itemCodeableConcept</t>
+  </si>
+  <si>
+    <t>Coded Ingredient Product</t>
+  </si>
+  <si>
+    <t>Coding for a substance or medicinal product  that is an ingredient of the medication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org.au/fhir/ValueSet/amt-mp-codes</t>
   </si>
   <si>
     <t>Medication.ingredient.isActive</t>
@@ -7984,13 +7984,13 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>118</v>
+        <v>275</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8017,11 +8017,13 @@
         <v>40</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="X61" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y61" t="s" s="2">
-        <v>277</v>
+        <v>40</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>40</v>
@@ -8071,7 +8073,7 @@
         <v>266</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C62" t="s" s="2">
         <v>40</v>
@@ -8093,13 +8095,13 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8126,13 +8128,11 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="X62" s="2"/>
       <c r="Y62" t="s" s="2">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>40</v>

</xml_diff>